<commit_message>
Add CSV data file
</commit_message>
<xml_diff>
--- a/app/argo_dummy.xlsx
+++ b/app/argo_dummy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b5c6bdd4f01e3a90/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\floatchat-backend\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E304EF0B-FAB5-41E0-92E3-7A13AB928772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B6F3E5-E10C-410D-AE09-0EA91B8B71F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9575098C-5056-4280-B4A1-8B275B402B58}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{9575098C-5056-4280-B4A1-8B275B402B58}"/>
   </bookViews>
   <sheets>
     <sheet name="argo_dummy" sheetId="1" r:id="rId1"/>
@@ -931,7 +931,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E4BDFD-2ECF-4560-95BF-04E9CD918A65}">
   <dimension ref="A1:H251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>